<commit_message>
Add LoginUserDto for login status check + TODOs + Admin functionalities planned
</commit_message>
<xml_diff>
--- a/SquashPlanner.xlsx
+++ b/SquashPlanner.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="324" yWindow="612" windowWidth="10236" windowHeight="2076" activeTab="3"/>
+    <workbookView xWindow="324" yWindow="612" windowWidth="10236" windowHeight="2076" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DB" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="91">
   <si>
     <t>Honnan (HTML)</t>
   </si>
@@ -282,6 +282,52 @@
   </si>
   <si>
     <t>Database</t>
+  </si>
+  <si>
+    <t>AdminDto</t>
+  </si>
+  <si>
+    <t>/admin/reg/user</t>
+  </si>
+  <si>
+    <t>Register new User</t>
+  </si>
+  <si>
+    <t>userId
+newUserName
+newUserRole</t>
+  </si>
+  <si>
+    <t>/admin/reg/place</t>
+  </si>
+  <si>
+    <t>Register new Place</t>
+  </si>
+  <si>
+    <t>userId
+newPlaceName
+newPlacePrice
+newPlaceAddress</t>
+  </si>
+  <si>
+    <t>/admin/reg/game</t>
+  </si>
+  <si>
+    <t>Register new Game</t>
+  </si>
+  <si>
+    <t>userId
+newUser1Id
+newUser1Points
+newUser2Id
+newUser2Points
+newPlaceId
+newDate</t>
+  </si>
+  <si>
+    <t>userid::int
+allUsers::List&lt;UserDto&gt;
+allPlaces::List&lt;PlaceDto&gt;</t>
   </si>
 </sst>
 </file>
@@ -293,6 +339,14 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -346,16 +400,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7030A0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -461,39 +505,67 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -501,17 +573,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -722,7 +784,7 @@
   <dimension ref="A1:D974"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -736,7 +798,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="22" t="s">
         <v>14</v>
       </c>
       <c r="B1" s="7" t="s">
@@ -750,7 +812,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A2" s="8"/>
+      <c r="A2" s="22"/>
       <c r="B2" s="7" t="s">
         <v>18</v>
       </c>
@@ -759,7 +821,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A3" s="8"/>
+      <c r="A3" s="22"/>
       <c r="B3" s="7" t="s">
         <v>19</v>
       </c>
@@ -768,7 +830,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A4" s="8"/>
+      <c r="A4" s="22"/>
       <c r="B4" s="7" t="s">
         <v>20</v>
       </c>
@@ -777,7 +839,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A5" s="8"/>
+      <c r="A5" s="22"/>
       <c r="B5" s="7" t="s">
         <v>21</v>
       </c>
@@ -786,17 +848,17 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A6" s="8"/>
-      <c r="B6" s="9" t="s">
+      <c r="A6" s="22"/>
+      <c r="B6" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="11"/>
+      <c r="D6" s="10"/>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="22" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="7" t="s">
@@ -810,7 +872,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A8" s="8"/>
+      <c r="A8" s="22"/>
       <c r="B8" s="7" t="s">
         <v>18</v>
       </c>
@@ -819,7 +881,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A9" s="8"/>
+      <c r="A9" s="22"/>
       <c r="B9" s="7" t="s">
         <v>26</v>
       </c>
@@ -828,17 +890,17 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A10" s="8"/>
-      <c r="B10" s="9" t="s">
+      <c r="A10" s="22"/>
+      <c r="B10" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="11"/>
+      <c r="D10" s="10"/>
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="22" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="7" t="s">
@@ -852,7 +914,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A12" s="8"/>
+      <c r="A12" s="22"/>
       <c r="B12" s="7" t="s">
         <v>29</v>
       </c>
@@ -864,7 +926,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A13" s="8"/>
+      <c r="A13" s="22"/>
       <c r="B13" s="7" t="s">
         <v>34</v>
       </c>
@@ -874,7 +936,7 @@
       <c r="D13" s="7"/>
     </row>
     <row r="14" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A14" s="8"/>
+      <c r="A14" s="22"/>
       <c r="B14" s="7" t="s">
         <v>30</v>
       </c>
@@ -886,7 +948,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A15" s="8"/>
+      <c r="A15" s="22"/>
       <c r="B15" s="7" t="s">
         <v>35</v>
       </c>
@@ -896,7 +958,7 @@
       <c r="D15" s="7"/>
     </row>
     <row r="16" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A16" s="8"/>
+      <c r="A16" s="22"/>
       <c r="B16" s="7" t="s">
         <v>32</v>
       </c>
@@ -908,27 +970,27 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A17" s="8"/>
-      <c r="B17" s="9" t="s">
+      <c r="A17" s="22"/>
+      <c r="B17" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="11"/>
+      <c r="D17" s="10"/>
     </row>
     <row r="18" spans="1:4" ht="15.75" customHeight="1"/>
     <row r="19" spans="1:4" ht="15.75" customHeight="1"/>
     <row r="20" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A20" s="22" t="s">
+      <c r="A20" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="11" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.75" customHeight="1">
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="11" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1900,8 +1962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H998"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1942,200 +2004,202 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="15" customFormat="1" ht="14.4">
-      <c r="A2" s="16" t="s">
+    <row r="2" spans="1:8" s="14" customFormat="1" ht="14.4">
+      <c r="A2" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="15" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="12" customFormat="1" ht="63" customHeight="1">
-      <c r="A3" s="13" t="s">
+    <row r="3" spans="1:8" s="11" customFormat="1" ht="63" customHeight="1">
+      <c r="A3" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H3" s="12" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="12" customFormat="1" ht="63" customHeight="1">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="13" t="s">
+    <row r="4" spans="1:8" s="11" customFormat="1" ht="63" customHeight="1">
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="H4" s="12" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="12" customFormat="1" ht="63" customHeight="1">
-      <c r="A5" s="13"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="13" t="s">
+    <row r="5" spans="1:8" s="11" customFormat="1" ht="63" customHeight="1">
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="12" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="12" customFormat="1" ht="63" customHeight="1">
-      <c r="A6" s="13"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="13" t="s">
+    <row r="6" spans="1:8" s="11" customFormat="1" ht="63" customHeight="1">
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="G6" s="21"/>
-      <c r="H6" s="13" t="s">
+      <c r="G6" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="H6" s="12" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="12" customFormat="1" ht="63" customHeight="1">
-      <c r="A7" s="13" t="s">
+    <row r="7" spans="1:8" s="11" customFormat="1" ht="63" customHeight="1">
+      <c r="A7" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="H7" s="13" t="s">
+      <c r="H7" s="12" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="12" customFormat="1" ht="63" customHeight="1">
-      <c r="A8" s="13"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="13" t="s">
+    <row r="8" spans="1:8" s="11" customFormat="1" ht="63" customHeight="1">
+      <c r="A8" s="12"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="G8" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="H8" s="13" t="s">
+      <c r="H8" s="12" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="12" customFormat="1" ht="63" customHeight="1">
-      <c r="A9" s="13" t="s">
+    <row r="9" spans="1:8" s="11" customFormat="1" ht="63" customHeight="1">
+      <c r="A9" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="E9" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="G9" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="H9" s="13" t="s">
+      <c r="H9" s="12" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="12" customFormat="1" ht="63" customHeight="1">
-      <c r="A10" s="13" t="s">
+    <row r="10" spans="1:8" s="11" customFormat="1" ht="63" customHeight="1">
+      <c r="A10" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="E10" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="F10" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="G10" s="13" t="s">
+      <c r="G10" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="H10" s="13" t="s">
+      <c r="H10" s="12" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="12" customFormat="1" ht="14.4">
-      <c r="B11" s="14"/>
+    <row r="11" spans="1:8" s="11" customFormat="1" ht="14.4">
+      <c r="B11" s="13"/>
     </row>
     <row r="12" spans="1:8" ht="14.4">
       <c r="A12" s="3"/>
@@ -2150,30 +2214,92 @@
     <row r="13" spans="1:8" ht="14.4">
       <c r="B13" s="2"/>
     </row>
-    <row r="14" spans="1:8" ht="14.4">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-    </row>
-    <row r="15" spans="1:8" ht="14.4">
-      <c r="B15" s="2"/>
-    </row>
-    <row r="16" spans="1:8" ht="14.4">
-      <c r="B16" s="2"/>
+    <row r="14" spans="1:8" ht="65.400000000000006" customHeight="1">
+      <c r="A14" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="97.2" customHeight="1">
+      <c r="A15" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="E15" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="115.8" customHeight="1">
+      <c r="A16" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="E16" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="17" spans="2:2" ht="14.4">
-      <c r="B17" s="2"/>
+      <c r="B17" s="25"/>
     </row>
     <row r="18" spans="2:2" ht="14.4">
-      <c r="B18" s="2"/>
+      <c r="B18" s="25"/>
     </row>
     <row r="19" spans="2:2" ht="15.75" customHeight="1">
-      <c r="B19" s="2"/>
+      <c r="B19" s="25"/>
     </row>
     <row r="20" spans="2:2" ht="15.75" customHeight="1">
       <c r="B20" s="2"/>
@@ -5120,15 +5246,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="41.33203125" style="20" customWidth="1"/>
+    <col min="1" max="1" width="41.33203125" style="19" customWidth="1"/>
     <col min="2" max="2" width="41.33203125" customWidth="1"/>
     <col min="3" max="3" width="28.44140625" customWidth="1"/>
   </cols>
@@ -5140,73 +5266,84 @@
       <c r="B1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="21" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="33" customHeight="1" thickTop="1">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="61.2" customHeight="1">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="11" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="77.400000000000006" customHeight="1">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="11" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="175.8" customHeight="1">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="64.8" customHeight="1">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="11" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="52.2" customHeight="1">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="68.400000000000006" customHeight="1">
+      <c r="A8" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="29" t="s">
         <v>73</v>
       </c>
     </row>
@@ -5220,7 +5357,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C986"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -6256,42 +6393,42 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="15" customHeight="1">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" customHeight="1">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="12" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.4">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="12" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15" customHeight="1">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="11" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15" customHeight="1">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="11" t="s">
         <v>73</v>
       </c>
     </row>

</xml_diff>